<commit_message>
Add new line to comment excel sheet
</commit_message>
<xml_diff>
--- a/batch_files/issue_batch.xlsx
+++ b/batch_files/issue_batch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovannoni/code/github-issue-handler/batch_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6397F415-5879-6A4D-A794-7EE354CBADB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75634D74-4D3C-B84D-85C6-D6CE942620AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{458D60C4-FB36-1F42-A7E9-2E2806A02E66}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Issue ID</t>
   </si>
@@ -91,10 +91,13 @@
     <t>Add excel file parsing</t>
   </si>
   <si>
-    <t>test comment</t>
-  </si>
-  <si>
     <t>is this still open?</t>
+  </si>
+  <si>
+    <t>Wohooo</t>
+  </si>
+  <si>
+    <t>old school cool</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6784E057-36E7-F44E-8D71-515263C7B2A3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,10 +603,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BEE545-BE86-CA46-AF06-074AE8D7D9CD}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +639,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -644,10 +647,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[WIP] add text to pdf screenshot
</commit_message>
<xml_diff>
--- a/batch_files/issue_batch.xlsx
+++ b/batch_files/issue_batch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovannoni/code/github-issue-handler/batch_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75634D74-4D3C-B84D-85C6-D6CE942620AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829E885-07E5-F240-BF11-7ACB7F931474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{458D60C4-FB36-1F42-A7E9-2E2806A02E66}"/>
   </bookViews>
@@ -606,7 +606,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,6 +641,9 @@
       <c r="B2" t="s">
         <v>19</v>
       </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -649,6 +652,9 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -656,6 +662,9 @@
       </c>
       <c r="B4" t="s">
         <v>20</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructure project into packages (fixes #10)
</commit_message>
<xml_diff>
--- a/batch_files/issue_batch.xlsx
+++ b/batch_files/issue_batch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovannoni/code/github-issue-handler/batch_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829E885-07E5-F240-BF11-7ACB7F931474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25316D52-7EED-C64D-A5C0-F6D88EFB3767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{458D60C4-FB36-1F42-A7E9-2E2806A02E66}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +606,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>